<commit_message>
w2d3 - practice and exercise notes
</commit_message>
<xml_diff>
--- a/week_2/spreadsheets/day_3_exercise.xlsx
+++ b/week_2/spreadsheets/day_3_exercise.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,126 +424,126 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>528475</t>
+          <t>889104</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Sherlock</t>
+          <t>Guy</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Shakespeare</t>
+          <t>Dumas</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>538931</t>
+          <t>433402</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Guy</t>
+          <t>Ayn</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Rand</t>
+          <t>Sawyer</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>406208</t>
+          <t>216873</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Ayn</t>
+          <t>Guy</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Asimov</t>
+          <t>Holmes</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>779071</t>
+          <t>981322</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>William</t>
+          <t>Isaac</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Asimov</t>
+          <t>Montag</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>580372</t>
+          <t>562190</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Guy</t>
+          <t>Tom</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Rand</t>
+          <t>Holmes</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>312684</t>
+          <t>593299</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>William</t>
+          <t>Sherlock</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Dumas</t>
+          <t>Alighieri</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>607353</t>
+          <t>830210</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>William</t>
+          <t>Tom</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Asimov</t>
+          <t>Montag</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>851104</t>
+          <t>539227</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -553,24 +553,41 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Dumas</t>
+          <t>Sawyer</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>936695</t>
+          <t>350556</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Ayn</t>
+          <t>William</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Rand</t>
+          <t>Sanderson</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>244761</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Alexandre</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Sawyer</t>
         </is>
       </c>
     </row>

</xml_diff>